<commit_message>
added culture data browsing functinos
</commit_message>
<xml_diff>
--- a/media/dna_data.xlsx
+++ b/media/dna_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
-  <si>
-    <t>This file will be used to upload data to the NelsonDB. Field names should not be modified.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>Authored 03/04/2015</t>
   </si>
@@ -48,13 +45,7 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>lab_obsother</t>
-  </si>
-  <si>
     <t>Source Seed ID</t>
-  </si>
-  <si>
-    <t>source_stock = Stock(seed_id).id</t>
   </si>
   <si>
     <t>If the sample was selected using seed, provide the Seed ID here. If not applicable, leave blank.</t>
@@ -63,16 +54,10 @@
     <t>Source Isolate ID</t>
   </si>
   <si>
-    <t>source_isolate = Isolate(isolate_id).id</t>
-  </si>
-  <si>
     <t>If the sample was selected using an isolate, provide te isolate ID here. If not applicable leave blank.</t>
   </si>
   <si>
     <t>Source Row ID</t>
-  </si>
-  <si>
-    <t>source_row = ObsRow(row_id).id</t>
   </si>
   <si>
     <t>If the sample was selected from a row, provide the Row ID here. If not applicable, leave blank.</t>
@@ -81,16 +66,10 @@
     <t>Source Plant ID</t>
   </si>
   <si>
-    <t>source_plant = ObsPlant(plant_id).id</t>
-  </si>
-  <si>
     <t>If the sample was selected from a plant, provide the Plant ID here. If not applicable, leave blank.</t>
   </si>
   <si>
     <t>Source Well ID</t>
-  </si>
-  <si>
-    <t>source_well = ObsOther(well_id).id</t>
   </si>
   <si>
     <t>If the sample was selected from a specific well, provide the Well ID here. If not applicable, leave blank.</t>
@@ -99,16 +78,10 @@
     <t>Source Microbe ID</t>
   </si>
   <si>
-    <t>source_microbe = ObsOther(microbe_id).id</t>
-  </si>
-  <si>
     <t>If the sample was selected from a microbe, provide the Microbe ID here. If not applicable, leave blank.</t>
   </si>
   <si>
     <t>Source Culture ID</t>
-  </si>
-  <si>
-    <t>source_culture = ObsOther(culture_id).id</t>
   </si>
   <si>
     <t>If the sample was selected from a separate culture, provide the Culture ID here. If not applicable, leave blank.</t>
@@ -117,16 +90,10 @@
     <t>Source Tissue ID</t>
   </si>
   <si>
-    <t>source_tissue = ObsOther(tissue_id).id</t>
-  </si>
-  <si>
     <t>If the sample was selected from a tissue, provide the Tissue ID here. If not applicable, leave blank.</t>
   </si>
   <si>
     <t>Source Sample ID</t>
-  </si>
-  <si>
-    <t>source_sample = ObsOther(sample_id).id</t>
   </si>
   <si>
     <t>If the sample was selected from a specific sample, provide Sample ID here. If not applicable, leave blank.</t>
@@ -135,16 +102,10 @@
     <t>Source Plate ID</t>
   </si>
   <si>
-    <t>source_plate = ObsOther(plate_id).id</t>
-  </si>
-  <si>
     <t>If the sample was selected from a specific plate, provide the Plate ID here. If not applicable leave blank.</t>
   </si>
   <si>
     <t>Source DNA iD</t>
-  </si>
-  <si>
-    <t>source_dna = ObsOther(dna_id).id</t>
   </si>
   <si>
     <t xml:space="preserve">If the sample was selected from specific DNA, provide the DNA ID here. If not applicable, leave blank. </t>
@@ -175,21 +136,6 @@
   </si>
   <si>
     <t>dna_id</t>
-  </si>
-  <si>
-    <t>dna_extraction_method</t>
-  </si>
-  <si>
-    <t>dna_date</t>
-  </si>
-  <si>
-    <t>dna_tube_id</t>
-  </si>
-  <si>
-    <t>dna_tube_type</t>
-  </si>
-  <si>
-    <t>dna_comments</t>
   </si>
   <si>
     <t>Any additional comments about the DNA.</t>
@@ -231,12 +177,82 @@
   <si>
     <t>DNA Info</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This file will be used to upload data to the NelsonDB. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FIELD NAMES CAN BE ADDED, BUT SHOULD BE DONE SPARINGLY</t>
+    </r>
+  </si>
+  <si>
+    <t>lab_obsdna</t>
+  </si>
+  <si>
+    <t>extraction_method</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>tube_id</t>
+  </si>
+  <si>
+    <t>tube_type</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>lab_obstracker</t>
+  </si>
+  <si>
+    <t>stock_id = Stock(seed_id).id</t>
+  </si>
+  <si>
+    <t>isolate_id = Isolate(isolate_id).id</t>
+  </si>
+  <si>
+    <t>obs_row_id = ObsRow(row_id).id</t>
+  </si>
+  <si>
+    <t>obs_plant_id = ObsPlant(plant_id).id</t>
+  </si>
+  <si>
+    <t>obs_well_id = ObsWellr(well_id).id</t>
+  </si>
+  <si>
+    <t>obs_microbe_id = ObsMicrobe(microbe_id).id</t>
+  </si>
+  <si>
+    <t>obs_culture_id = ObsCulture(culture_id).id</t>
+  </si>
+  <si>
+    <t>obs_tissue_id = ObsTissue(tissue_id).id</t>
+  </si>
+  <si>
+    <t>obs_sample_id = ObsSample(sample_id).id</t>
+  </si>
+  <si>
+    <t>obs-plate_id = ObsPlate(plate_id).id</t>
+  </si>
+  <si>
+    <t>obs_dna_id = ObsDNA(dna_id).id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +295,14 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -693,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,279 +731,279 @@
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>2</v>
+      <c r="B16" s="5" t="s">
+        <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>3</v>
+      <c r="C16" t="s">
+        <v>52</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
+      <c r="D16" t="s">
+        <v>37</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
+      <c r="B18" s="5" t="s">
+        <v>53</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
-        <v>49</v>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>8</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
+      <c r="D20" t="s">
+        <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>7</v>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>50</v>
+      <c r="B21" s="5" t="s">
+        <v>53</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C21" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
+      <c r="D21" t="s">
+        <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>51</v>
+      <c r="B22" s="5" t="s">
+        <v>53</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>46</v>
+      <c r="D22" t="s">
+        <v>15</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>7</v>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>16</v>
       </c>
-      <c r="C14" t="s">
-        <v>52</v>
+      <c r="B23" s="5" t="s">
+        <v>53</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>47</v>
+      <c r="D23" t="s">
+        <v>17</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>7</v>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>18</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C24" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>7</v>
+      <c r="B25" s="5" t="s">
+        <v>53</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
         <v>21</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="B26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D23" t="s">
+      <c r="B27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="B28" s="5" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -991,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,14 +1042,14 @@
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1"/>
       <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2"/>
       <c r="Q2" s="6"/>
@@ -1038,7 +1062,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1059,55 +1083,55 @@
     </row>
     <row r="6" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>11</v>
+      <c r="I6" s="10" t="s">
+        <v>10</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="J6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="10" t="s">
-        <v>17</v>
+      <c r="L6" s="10" t="s">
+        <v>16</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="M6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="O6" s="10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>